<commit_message>
prepare fot Ver 1.1
</commit_message>
<xml_diff>
--- a/Assets/Trionfi/Documents/TagReference.xlsx
+++ b/Assets/Trionfi/Documents/TagReference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\井筒　紗奈\Desktop\Trionfi\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6070168ee4f0faf2/デスクトップ/Trionfi/Assets/Trionfi/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D811428A-0673-48AB-B311-90C8E17C9ACC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{D811428A-0673-48AB-B311-90C8E17C9ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9408024-026E-4DED-93C6-5366F6E34817}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{7F702E2A-9EB7-4142-98AC-0C9039DFE745}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7F702E2A-9EB7-4142-98AC-0C9039DFE745}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="154">
   <si>
     <t>タグ名</t>
     <rPh sb="2" eb="3">
@@ -1101,6 +1101,13 @@
     </rPh>
     <rPh sb="21" eb="23">
       <t>フヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>機能</t>
+    <rPh sb="0" eb="2">
+      <t>キノウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1109,7 +1116,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1125,6 +1132,15 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1134,12 +1150,21 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1148,11 +1173,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1471,8 +1499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A7694E-C34A-4AF6-AD55-184CC16CE10F}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1487,30 +1515,34 @@
     <col min="8" max="8" width="35.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B1" t="s">
+    <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="19.5" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>26</v>
       </c>

</xml_diff>